<commit_message>
Updated documentation and updated index1.php to index.php
</commit_message>
<xml_diff>
--- a/documentation/TestPlan (2).xlsx
+++ b/documentation/TestPlan (2).xlsx
@@ -17,12 +17,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
   <si>
     <t>and.h</t>
   </si>
@@ -192,9 +191,6 @@
     <t xml:space="preserve">User Information entered </t>
   </si>
   <si>
-    <t>User access granted</t>
-  </si>
-  <si>
     <t>Enter correct username and password</t>
   </si>
   <si>
@@ -256,6 +252,63 @@
   </si>
   <si>
     <t>User Registration/Login Display button clicked</t>
+  </si>
+  <si>
+    <t>Main Page appears with profile dropdown allowing login</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>User registeration form appears</t>
+  </si>
+  <si>
+    <t>User information sent to database</t>
+  </si>
+  <si>
+    <t>User information is in the database</t>
+  </si>
+  <si>
+    <t>Submit User registration</t>
+  </si>
+  <si>
+    <t>Succes or fail page is presented to user</t>
+  </si>
+  <si>
+    <t>Blank Screen</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Error page is displayed</t>
+  </si>
+  <si>
+    <t>Provides Success page but redirect doesn't work</t>
+  </si>
+  <si>
+    <t>User avatar(if set) shows up with text message</t>
+  </si>
+  <si>
+    <t>Second User avatar (if set) show up with text message on refresh</t>
+  </si>
+  <si>
+    <t>Upload avatar adds picture next to the username on toolbar and popup icon</t>
+  </si>
+  <si>
+    <t>Error page is displayed but bootstrap is not applied</t>
+  </si>
+  <si>
+    <t>Logout destroys session and can not access parts of the web site</t>
+  </si>
+  <si>
+    <t>Click About Page</t>
+  </si>
+  <si>
+    <t>Display information about the web page</t>
+  </si>
+  <si>
+    <t>Information is displayed about the web page</t>
   </si>
 </sst>
 </file>
@@ -543,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -587,6 +640,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -744,7 +798,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A9:F22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A9:F23">
   <tableColumns count="6">
     <tableColumn id="1" name="#"/>
     <tableColumn id="2" name="Date"/>
@@ -1054,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH1000"/>
+  <dimension ref="A1:AH1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -1073,22 +1127,22 @@
   <sheetData>
     <row r="1" spans="1:34" ht="23.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:34">
@@ -1097,7 +1151,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>25</v>
@@ -1132,7 +1186,9 @@
       <c r="D5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="16"/>
+      <c r="E5" s="16">
+        <v>42587</v>
+      </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:34">
@@ -1146,7 +1202,9 @@
       <c r="D6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="16"/>
+      <c r="E6" s="16">
+        <v>42952</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:34" ht="15.75" customHeight="1">
@@ -1200,8 +1258,12 @@
       <c r="D10" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="28"/>
+      <c r="E10" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="11" spans="1:34" ht="30" customHeight="1">
       <c r="A11" s="25">
@@ -1209,13 +1271,17 @@
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>78</v>
+      </c>
       <c r="I11" s="29"/>
       <c r="J11" s="29"/>
       <c r="K11" s="29"/>
@@ -1243,7 +1309,7 @@
       <c r="AG11" s="30"/>
       <c r="AH11" s="30"/>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:34" ht="30">
       <c r="A12" s="28">
         <v>3</v>
       </c>
@@ -1252,154 +1318,210 @@
         <v>55</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="25"/>
-    </row>
-    <row r="13" spans="1:34" ht="30">
-      <c r="A13" s="28">
-        <v>4</v>
+      <c r="E12" s="27" t="s">
+        <v>81</v>
       </c>
+      <c r="F12" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" s="31" customFormat="1" ht="30">
+      <c r="A13" s="28"/>
       <c r="B13" s="26"/>
       <c r="C13" s="27" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="25"/>
-    </row>
-    <row r="14" spans="1:34">
+      <c r="E13" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="30">
       <c r="A14" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="25"/>
-    </row>
-    <row r="15" spans="1:34" ht="30" customHeight="1">
+      <c r="E14" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34">
       <c r="A15" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="25"/>
+      <c r="E15" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="16" spans="1:34" ht="30" customHeight="1">
       <c r="A16" s="28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="25"/>
+      <c r="E16" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1">
       <c r="A17" s="28">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1">
       <c r="A18" s="28">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="27" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="25"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="E18" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1">
       <c r="A19" s="28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="26"/>
       <c r="C19" s="27" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="25"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1">
+      <c r="E19" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="28">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="25"/>
-    </row>
-    <row r="21" spans="1:6" ht="30">
+      <c r="E20" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1">
       <c r="A21" s="28">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30">
+      <c r="A22" s="28">
+        <v>12</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="27" t="s">
-        <v>75</v>
+      <c r="E22" s="27" t="s">
+        <v>92</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="25"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="25">
+      <c r="F22" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30">
+      <c r="A23" s="25">
         <v>13</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="25"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1"/>
@@ -9217,17 +9339,25 @@
       <c r="E1000" s="1"/>
       <c r="F1000" s="1"/>
     </row>
+    <row r="1001" spans="1:6">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="1"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F10:F22">
+  <conditionalFormatting sqref="F10:F23">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F22">
+  <conditionalFormatting sqref="F10:F23">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>

</xml_diff>